<commit_message>
- Finished adaptation to JMS board footprint. - Added testpoints. - Changed header connector to 0.1" pitch, and tall.
</commit_message>
<xml_diff>
--- a/Gerbers/Bill of Materials.xlsx
+++ b/Gerbers/Bill of Materials.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtetil\Documents\Projects\hp-bldc-pcb\Gerbers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="150" yWindow="570" windowWidth="28455" windowHeight="11955"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="BOM v1.0" sheetId="1" r:id="rId1"/>
@@ -386,27 +391,27 @@
     <t>L101</t>
   </si>
   <si>
-    <t>M40-3200645R</t>
-  </si>
-  <si>
-    <t>CONN HEADER 12POS 1MM DL AU SMD</t>
-  </si>
-  <si>
-    <t>HARWIN</t>
-  </si>
-  <si>
     <t>ST401</t>
+  </si>
+  <si>
+    <t>TSM-105-03-T-SV</t>
+  </si>
+  <si>
+    <t>CONN HEADER 5POS 0.1" SMD</t>
+  </si>
+  <si>
+    <t>SAMTEC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="#,##0.0"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -687,6 +692,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -733,7 +746,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -765,9 +778,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -799,6 +813,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -974,14 +989,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="5.7109375" customWidth="1"/>
@@ -991,7 +1006,7 @@
     <col min="6" max="6" width="39.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.75">
+    <row r="1" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -1011,7 +1026,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="12.75">
+    <row r="2" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="36">
         <v>1</v>
       </c>
@@ -1031,7 +1046,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="12.75">
+    <row r="3" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="36">
         <v>2</v>
       </c>
@@ -1051,7 +1066,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="12.75">
+    <row r="4" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="36">
         <v>3</v>
       </c>
@@ -1078,7 +1093,7 @@
       <c r="L4" s="41"/>
       <c r="M4" s="41"/>
     </row>
-    <row r="5" spans="1:13" ht="25.5">
+    <row r="5" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A5" s="36">
         <v>4</v>
       </c>
@@ -1105,7 +1120,7 @@
       <c r="L5" s="41"/>
       <c r="M5" s="41"/>
     </row>
-    <row r="6" spans="1:13" ht="12.75">
+    <row r="6" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="36">
         <v>5</v>
       </c>
@@ -1125,7 +1140,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="12.75">
+    <row r="7" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="36">
         <v>6</v>
       </c>
@@ -1145,7 +1160,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="25.5">
+    <row r="8" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A8" s="36">
         <v>7</v>
       </c>
@@ -1165,7 +1180,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="12.75">
+    <row r="9" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
         <v>8</v>
       </c>
@@ -1185,7 +1200,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="12.75">
+    <row r="10" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="36">
         <v>9</v>
       </c>
@@ -1205,7 +1220,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="12.75">
+    <row r="11" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
         <v>10</v>
       </c>
@@ -1225,7 +1240,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="12.75">
+    <row r="12" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="36">
         <v>11</v>
       </c>
@@ -1245,7 +1260,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="12.75">
+    <row r="13" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="36">
         <v>12</v>
       </c>
@@ -1265,7 +1280,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="12.75">
+    <row r="14" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="36">
         <v>13</v>
       </c>
@@ -1285,7 +1300,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="12.75">
+    <row r="15" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="36">
         <v>14</v>
       </c>
@@ -1305,7 +1320,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="12.75">
+    <row r="16" spans="1:13" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="36">
         <v>15</v>
       </c>
@@ -1325,7 +1340,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="12.75">
+    <row r="17" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="36">
         <v>16</v>
       </c>
@@ -1345,7 +1360,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="12.75">
+    <row r="18" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="36">
         <v>17</v>
       </c>
@@ -1365,7 +1380,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="12.75">
+    <row r="19" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A19" s="36">
         <v>18</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="12.75">
+    <row r="20" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A20" s="36">
         <v>19</v>
       </c>
@@ -1405,7 +1420,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="12.75">
+    <row r="21" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A21" s="36">
         <v>20</v>
       </c>
@@ -1425,7 +1440,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="12.75">
+    <row r="22" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A22" s="36">
         <v>21</v>
       </c>
@@ -1445,7 +1460,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="12.75">
+    <row r="23" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A23" s="36">
         <v>22</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="12.75">
+    <row r="24" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A24" s="36">
         <v>23</v>
       </c>
@@ -1485,7 +1500,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="12.75">
+    <row r="25" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A25" s="36">
         <v>24</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="12.75">
+    <row r="26" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A26" s="36">
         <v>25</v>
       </c>
@@ -1525,7 +1540,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="27" spans="1:6" ht="12.75">
+    <row r="27" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A27" s="36">
         <v>26</v>
       </c>
@@ -1545,7 +1560,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="12.75">
+    <row r="28" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A28" s="36">
         <v>27</v>
       </c>
@@ -1565,7 +1580,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="12.75">
+    <row r="29" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="36">
         <v>28</v>
       </c>
@@ -1585,7 +1600,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="12.75">
+    <row r="30" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="36">
         <v>29</v>
       </c>
@@ -1605,7 +1620,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="12.75">
+    <row r="31" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="36">
         <v>30</v>
       </c>
@@ -1625,7 +1640,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="12.75">
+    <row r="32" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="36">
         <v>31</v>
       </c>
@@ -1645,7 +1660,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="12.75">
+    <row r="33" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="36">
         <v>32</v>
       </c>
@@ -1665,7 +1680,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="12.75">
+    <row r="34" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="36">
         <v>33</v>
       </c>
@@ -1685,7 +1700,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="12.75">
+    <row r="35" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="36">
         <v>34</v>
       </c>
@@ -1693,19 +1708,19 @@
         <v>1</v>
       </c>
       <c r="C35" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="F35" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D35" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="E35" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F35" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="12.75">
+    </row>
+    <row r="36" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="36">
         <v>35</v>
       </c>
@@ -1715,7 +1730,7 @@
       <c r="E36" s="10"/>
       <c r="F36" s="10"/>
     </row>
-    <row r="37" spans="1:6" ht="12.75">
+    <row r="37" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="36">
         <v>36</v>
       </c>
@@ -1725,7 +1740,7 @@
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
     </row>
-    <row r="38" spans="1:6" ht="12.75">
+    <row r="38" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="36">
         <v>37</v>
       </c>
@@ -1735,7 +1750,7 @@
       <c r="E38" s="10"/>
       <c r="F38" s="43"/>
     </row>
-    <row r="39" spans="1:6" ht="12.75">
+    <row r="39" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="36">
         <v>38</v>
       </c>
@@ -1745,7 +1760,7 @@
       <c r="E39" s="27"/>
       <c r="F39" s="10"/>
     </row>
-    <row r="40" spans="1:6" ht="12.75">
+    <row r="40" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="36">
         <v>39</v>
       </c>
@@ -1755,7 +1770,7 @@
       <c r="E40" s="10"/>
       <c r="F40" s="10"/>
     </row>
-    <row r="41" spans="1:6" ht="12.75">
+    <row r="41" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="36">
         <v>40</v>
       </c>
@@ -1765,7 +1780,7 @@
       <c r="E41" s="10"/>
       <c r="F41" s="10"/>
     </row>
-    <row r="42" spans="1:6" ht="12.75">
+    <row r="42" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="36">
         <v>41</v>
       </c>
@@ -1775,7 +1790,7 @@
       <c r="E42" s="27"/>
       <c r="F42" s="27"/>
     </row>
-    <row r="43" spans="1:6" ht="12.75">
+    <row r="43" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="36">
         <v>42</v>
       </c>
@@ -1785,7 +1800,7 @@
       <c r="E43" s="10"/>
       <c r="F43" s="10"/>
     </row>
-    <row r="44" spans="1:6" ht="12.75">
+    <row r="44" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="36">
         <v>43</v>
       </c>
@@ -1795,7 +1810,7 @@
       <c r="E44" s="10"/>
       <c r="F44" s="10"/>
     </row>
-    <row r="45" spans="1:6" ht="12.75">
+    <row r="45" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="36">
         <v>44</v>
       </c>
@@ -1805,7 +1820,7 @@
       <c r="E45" s="10"/>
       <c r="F45" s="10"/>
     </row>
-    <row r="46" spans="1:6" ht="12.75">
+    <row r="46" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="36">
         <v>45</v>
       </c>
@@ -1815,7 +1830,7 @@
       <c r="E46" s="27"/>
       <c r="F46" s="27"/>
     </row>
-    <row r="47" spans="1:6" ht="12.75">
+    <row r="47" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="36">
         <v>46</v>
       </c>
@@ -1825,7 +1840,7 @@
       <c r="E47" s="10"/>
       <c r="F47" s="10"/>
     </row>
-    <row r="48" spans="1:6" ht="12.75">
+    <row r="48" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="36">
         <v>47</v>
       </c>
@@ -1835,7 +1850,7 @@
       <c r="E48" s="10"/>
       <c r="F48" s="10"/>
     </row>
-    <row r="49" spans="1:6" ht="12.75">
+    <row r="49" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="36">
         <v>48</v>
       </c>
@@ -1845,7 +1860,7 @@
       <c r="E49" s="10"/>
       <c r="F49" s="10"/>
     </row>
-    <row r="50" spans="1:6" ht="12.75">
+    <row r="50" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="36">
         <v>49</v>
       </c>
@@ -1855,7 +1870,7 @@
       <c r="E50" s="27"/>
       <c r="F50" s="27"/>
     </row>
-    <row r="51" spans="1:6" ht="12.75">
+    <row r="51" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="36">
         <v>50</v>
       </c>
@@ -1865,7 +1880,7 @@
       <c r="E51" s="10"/>
       <c r="F51" s="10"/>
     </row>
-    <row r="52" spans="1:6" ht="12.75">
+    <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="36">
         <v>51</v>
       </c>
@@ -1875,7 +1890,7 @@
       <c r="E52" s="10"/>
       <c r="F52" s="10"/>
     </row>
-    <row r="53" spans="1:6" ht="12.75">
+    <row r="53" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="36">
         <v>52</v>
       </c>
@@ -1885,7 +1900,7 @@
       <c r="E53" s="10"/>
       <c r="F53" s="10"/>
     </row>
-    <row r="54" spans="1:6" ht="12.75">
+    <row r="54" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="36">
         <v>53</v>
       </c>
@@ -1895,7 +1910,7 @@
       <c r="E54" s="10"/>
       <c r="F54" s="10"/>
     </row>
-    <row r="55" spans="1:6" ht="12.75">
+    <row r="55" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="36">
         <v>54</v>
       </c>
@@ -1905,7 +1920,7 @@
       <c r="E55" s="10"/>
       <c r="F55" s="10"/>
     </row>
-    <row r="56" spans="1:6" ht="12.75">
+    <row r="56" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="36">
         <v>55</v>
       </c>
@@ -1915,7 +1930,7 @@
       <c r="E56" s="10"/>
       <c r="F56" s="10"/>
     </row>
-    <row r="57" spans="1:6" ht="12.75">
+    <row r="57" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="36">
         <v>56</v>
       </c>
@@ -1925,7 +1940,7 @@
       <c r="E57" s="10"/>
       <c r="F57" s="10"/>
     </row>
-    <row r="58" spans="1:6" ht="12.75">
+    <row r="58" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="36">
         <v>57</v>
       </c>
@@ -1935,7 +1950,7 @@
       <c r="E58" s="10"/>
       <c r="F58" s="10"/>
     </row>
-    <row r="59" spans="1:6" ht="12.75">
+    <row r="59" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="36">
         <v>58</v>
       </c>
@@ -1945,7 +1960,7 @@
       <c r="E59" s="10"/>
       <c r="F59" s="10"/>
     </row>
-    <row r="60" spans="1:6" ht="12.75">
+    <row r="60" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="36">
         <v>59</v>
       </c>
@@ -1955,7 +1970,7 @@
       <c r="E60" s="10"/>
       <c r="F60" s="10"/>
     </row>
-    <row r="61" spans="1:6" ht="12.75">
+    <row r="61" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="36">
         <v>60</v>
       </c>
@@ -1965,7 +1980,7 @@
       <c r="E61" s="10"/>
       <c r="F61" s="10"/>
     </row>
-    <row r="62" spans="1:6" ht="12.75">
+    <row r="62" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="36">
         <v>61</v>
       </c>
@@ -1975,7 +1990,7 @@
       <c r="E62" s="10"/>
       <c r="F62" s="10"/>
     </row>
-    <row r="63" spans="1:6" ht="12.75">
+    <row r="63" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="36">
         <v>62</v>
       </c>
@@ -1985,7 +2000,7 @@
       <c r="E63" s="27"/>
       <c r="F63" s="27"/>
     </row>
-    <row r="64" spans="1:6" ht="12.75">
+    <row r="64" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="36">
         <v>63</v>
       </c>
@@ -1995,7 +2010,7 @@
       <c r="E64" s="10"/>
       <c r="F64" s="10"/>
     </row>
-    <row r="65" spans="1:6" ht="12.75">
+    <row r="65" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="36">
         <v>64</v>
       </c>
@@ -2005,7 +2020,7 @@
       <c r="E65" s="10"/>
       <c r="F65" s="10"/>
     </row>
-    <row r="66" spans="1:6" ht="12.75">
+    <row r="66" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="36">
         <v>65</v>
       </c>
@@ -2015,7 +2030,7 @@
       <c r="E66" s="10"/>
       <c r="F66" s="10"/>
     </row>
-    <row r="67" spans="1:6" ht="12.75">
+    <row r="67" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="36">
         <v>66</v>
       </c>
@@ -2025,7 +2040,7 @@
       <c r="E67" s="10"/>
       <c r="F67" s="10"/>
     </row>
-    <row r="68" spans="1:6" ht="12.75">
+    <row r="68" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="36">
         <v>67</v>
       </c>
@@ -2035,7 +2050,7 @@
       <c r="E68" s="10"/>
       <c r="F68" s="10"/>
     </row>
-    <row r="69" spans="1:6" ht="12.75">
+    <row r="69" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="36">
         <v>68</v>
       </c>
@@ -2045,7 +2060,7 @@
       <c r="E69" s="10"/>
       <c r="F69" s="10"/>
     </row>
-    <row r="70" spans="1:6" ht="12.75">
+    <row r="70" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="36">
         <v>69</v>
       </c>
@@ -2055,7 +2070,7 @@
       <c r="E70" s="10"/>
       <c r="F70" s="10"/>
     </row>
-    <row r="71" spans="1:6" ht="12.75">
+    <row r="71" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="36">
         <v>70</v>
       </c>
@@ -2065,7 +2080,7 @@
       <c r="E71" s="27"/>
       <c r="F71" s="27"/>
     </row>
-    <row r="72" spans="1:6" ht="12.75">
+    <row r="72" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="36">
         <v>71</v>
       </c>
@@ -2075,7 +2090,7 @@
       <c r="E72" s="10"/>
       <c r="F72" s="10"/>
     </row>
-    <row r="73" spans="1:6" ht="12.75">
+    <row r="73" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="36">
         <v>72</v>
       </c>
@@ -2085,14 +2100,14 @@
       <c r="E73" s="10"/>
       <c r="F73" s="10"/>
     </row>
-    <row r="74" spans="1:6" ht="12.75">
+    <row r="74" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="36">
         <v>73</v>
       </c>
       <c r="B74" s="12"/>
       <c r="C74" s="44"/>
     </row>
-    <row r="75" spans="1:6" ht="12.75">
+    <row r="75" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="36">
         <v>74</v>
       </c>
@@ -2102,7 +2117,7 @@
       <c r="E75" s="40"/>
       <c r="F75" s="40"/>
     </row>
-    <row r="76" spans="1:6" ht="12.75">
+    <row r="76" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="36">
         <v>75</v>
       </c>
@@ -2112,7 +2127,7 @@
       <c r="E76" s="40"/>
       <c r="F76" s="40"/>
     </row>
-    <row r="77" spans="1:6" ht="12.75">
+    <row r="77" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="36">
         <v>76</v>
       </c>
@@ -2122,7 +2137,7 @@
       <c r="E77" s="40"/>
       <c r="F77" s="40"/>
     </row>
-    <row r="78" spans="1:6" ht="12.75">
+    <row r="78" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="36">
         <v>77</v>
       </c>
@@ -2132,7 +2147,7 @@
       <c r="E78" s="40"/>
       <c r="F78" s="40"/>
     </row>
-    <row r="79" spans="1:6" ht="12.75">
+    <row r="79" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="36">
         <v>78</v>
       </c>
@@ -2142,7 +2157,7 @@
       <c r="E79" s="40"/>
       <c r="F79" s="40"/>
     </row>
-    <row r="80" spans="1:6" ht="12.75">
+    <row r="80" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="47"/>
       <c r="B80" s="45"/>
       <c r="C80" s="46"/>
@@ -2150,7 +2165,7 @@
       <c r="E80" s="40"/>
       <c r="F80" s="40"/>
     </row>
-    <row r="81" spans="1:6" ht="12.75">
+    <row r="81" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="47"/>
       <c r="B81" s="45"/>
       <c r="C81" s="46"/>
@@ -2158,7 +2173,7 @@
       <c r="E81" s="40"/>
       <c r="F81" s="40"/>
     </row>
-    <row r="82" spans="1:6" ht="12.75">
+    <row r="82" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="36"/>
       <c r="B82" s="37"/>
       <c r="C82" s="30"/>
@@ -2166,7 +2181,7 @@
       <c r="E82" s="10"/>
       <c r="F82" s="10"/>
     </row>
-    <row r="83" spans="1:6" ht="12.75">
+    <row r="83" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="36"/>
       <c r="B83" s="37"/>
       <c r="C83" s="30"/>
@@ -2174,7 +2189,7 @@
       <c r="E83" s="10"/>
       <c r="F83" s="10"/>
     </row>
-    <row r="84" spans="1:6" ht="12.75">
+    <row r="84" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="36"/>
       <c r="B84" s="37"/>
       <c r="C84" s="30"/>
@@ -2182,7 +2197,7 @@
       <c r="E84" s="10"/>
       <c r="F84" s="10"/>
     </row>
-    <row r="85" spans="1:6" ht="12.75">
+    <row r="85" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="36"/>
       <c r="B85" s="37"/>
       <c r="C85" s="30"/>
@@ -2190,12 +2205,12 @@
       <c r="E85" s="10"/>
       <c r="F85" s="10"/>
     </row>
-    <row r="86" spans="1:6" ht="12.75">
+    <row r="86" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="36"/>
       <c r="B86" s="42"/>
       <c r="F86" s="10"/>
     </row>
-    <row r="87" spans="1:6" ht="12.75">
+    <row r="87" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="48"/>
       <c r="B87" s="18"/>
       <c r="C87" s="49"/>
@@ -2205,22 +2220,23 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.85546875" customWidth="1"/>
     <col min="2" max="2" width="153" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2228,7 +2244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2237,308 +2253,308 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5"/>
       <c r="B3" s="6"/>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
       <c r="B4" s="8"/>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9"/>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="11"/>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="11"/>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="11"/>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="11"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
     </row>
-    <row r="17" spans="1:1" ht="15.75" customHeight="1">
+    <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
     </row>
-    <row r="18" spans="1:1" ht="15.75" customHeight="1">
+    <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
     </row>
-    <row r="19" spans="1:1" ht="15.75" customHeight="1">
+    <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
     </row>
-    <row r="20" spans="1:1" ht="15.75" customHeight="1">
+    <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11"/>
     </row>
-    <row r="21" spans="1:1" ht="15.75" customHeight="1">
+    <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
     </row>
-    <row r="22" spans="1:1" ht="15.75" customHeight="1">
+    <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
     </row>
-    <row r="23" spans="1:1" ht="15.75" customHeight="1">
+    <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
     </row>
-    <row r="24" spans="1:1" ht="15.75" customHeight="1">
+    <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
     </row>
-    <row r="25" spans="1:1" ht="15.75" customHeight="1">
+    <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
     </row>
-    <row r="26" spans="1:1" ht="15.75" customHeight="1">
+    <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
     </row>
-    <row r="27" spans="1:1" ht="15.75" customHeight="1">
+    <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
     </row>
-    <row r="28" spans="1:1" ht="15.75" customHeight="1">
+    <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
     </row>
-    <row r="29" spans="1:1" ht="15.75" customHeight="1">
+    <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
     </row>
-    <row r="30" spans="1:1" ht="15.75" customHeight="1">
+    <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
     </row>
-    <row r="31" spans="1:1" ht="15.75" customHeight="1">
+    <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
     </row>
-    <row r="32" spans="1:1" ht="15.75" customHeight="1">
+    <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
     </row>
-    <row r="33" spans="1:1" ht="15.75" customHeight="1">
+    <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
     </row>
-    <row r="34" spans="1:1" ht="15.75" customHeight="1">
+    <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
     </row>
-    <row r="35" spans="1:1" ht="15.75" customHeight="1">
+    <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
     </row>
-    <row r="36" spans="1:1" ht="15.75" customHeight="1">
+    <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
     </row>
-    <row r="37" spans="1:1" ht="15.75" customHeight="1">
+    <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
     </row>
-    <row r="38" spans="1:1" ht="15.75" customHeight="1">
+    <row r="38" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
     </row>
-    <row r="39" spans="1:1" ht="15.75" customHeight="1">
+    <row r="39" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
     </row>
-    <row r="40" spans="1:1" ht="15.75" customHeight="1">
+    <row r="40" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
     </row>
-    <row r="41" spans="1:1" ht="15.75" customHeight="1">
+    <row r="41" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
     </row>
-    <row r="42" spans="1:1" ht="15.75" customHeight="1">
+    <row r="42" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
     </row>
-    <row r="43" spans="1:1" ht="15.75" customHeight="1">
+    <row r="43" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
     </row>
-    <row r="44" spans="1:1" ht="15.75" customHeight="1">
+    <row r="44" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
     </row>
-    <row r="45" spans="1:1" ht="15.75" customHeight="1">
+    <row r="45" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
     </row>
-    <row r="46" spans="1:1" ht="15.75" customHeight="1">
+    <row r="46" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
     </row>
-    <row r="47" spans="1:1" ht="15.75" customHeight="1">
+    <row r="47" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
     </row>
-    <row r="48" spans="1:1" ht="15.75" customHeight="1">
+    <row r="48" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="12"/>
     </row>
-    <row r="49" spans="1:1" ht="15.75" customHeight="1">
+    <row r="49" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="12"/>
     </row>
-    <row r="50" spans="1:1" ht="15.75" customHeight="1">
+    <row r="50" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
     </row>
-    <row r="51" spans="1:1" ht="15.75" customHeight="1">
+    <row r="51" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
     </row>
-    <row r="52" spans="1:1" ht="15.75" customHeight="1">
+    <row r="52" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12"/>
     </row>
-    <row r="53" spans="1:1" ht="15.75" customHeight="1">
+    <row r="53" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12"/>
     </row>
-    <row r="54" spans="1:1" ht="15.75" customHeight="1">
+    <row r="54" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
     </row>
-    <row r="55" spans="1:1" ht="15.75" customHeight="1">
+    <row r="55" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="12"/>
     </row>
-    <row r="56" spans="1:1" ht="15.75" customHeight="1">
+    <row r="56" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="12"/>
     </row>
-    <row r="57" spans="1:1" ht="15.75" customHeight="1">
+    <row r="57" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12"/>
     </row>
-    <row r="58" spans="1:1" ht="15.75" customHeight="1">
+    <row r="58" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12"/>
     </row>
-    <row r="59" spans="1:1" ht="15.75" customHeight="1">
+    <row r="59" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
     </row>
-    <row r="60" spans="1:1" ht="15.75" customHeight="1">
+    <row r="60" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
     </row>
-    <row r="61" spans="1:1" ht="15.75" customHeight="1">
+    <row r="61" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
     </row>
-    <row r="62" spans="1:1" ht="15.75" customHeight="1">
+    <row r="62" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
     </row>
-    <row r="63" spans="1:1" ht="15.75" customHeight="1">
+    <row r="63" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12"/>
     </row>
-    <row r="64" spans="1:1" ht="15.75" customHeight="1">
+    <row r="64" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12"/>
     </row>
-    <row r="65" spans="1:1" ht="15.75" customHeight="1">
+    <row r="65" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12"/>
     </row>
-    <row r="66" spans="1:1" ht="15.75" customHeight="1">
+    <row r="66" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
     </row>
-    <row r="67" spans="1:1" ht="15.75" customHeight="1">
+    <row r="67" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
     </row>
-    <row r="68" spans="1:1" ht="15.75" customHeight="1">
+    <row r="68" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="12"/>
     </row>
-    <row r="69" spans="1:1" ht="15.75" customHeight="1">
+    <row r="69" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12"/>
     </row>
-    <row r="70" spans="1:1" ht="15.75" customHeight="1">
+    <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12"/>
     </row>
-    <row r="71" spans="1:1" ht="15.75" customHeight="1">
+    <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12"/>
     </row>
-    <row r="72" spans="1:1" ht="15.75" customHeight="1">
+    <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="12"/>
     </row>
-    <row r="73" spans="1:1" ht="15.75" customHeight="1">
+    <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="12"/>
     </row>
-    <row r="74" spans="1:1" ht="15.75" customHeight="1">
+    <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12"/>
     </row>
-    <row r="75" spans="1:1" ht="15.75" customHeight="1">
+    <row r="75" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12"/>
     </row>
-    <row r="76" spans="1:1" ht="15.75" customHeight="1">
+    <row r="76" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="12"/>
     </row>
-    <row r="77" spans="1:1" ht="15.75" customHeight="1">
+    <row r="77" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12"/>
     </row>
-    <row r="78" spans="1:1" ht="15.75" customHeight="1">
+    <row r="78" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12"/>
     </row>
-    <row r="79" spans="1:1" ht="15.75" customHeight="1">
+    <row r="79" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12"/>
     </row>
-    <row r="80" spans="1:1" ht="15.75" customHeight="1">
+    <row r="80" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12"/>
     </row>
-    <row r="81" spans="1:1" ht="15.75" customHeight="1">
+    <row r="81" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12"/>
     </row>
-    <row r="82" spans="1:1" ht="15.75" customHeight="1">
+    <row r="82" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12"/>
     </row>
-    <row r="83" spans="1:1" ht="15.75" customHeight="1">
+    <row r="83" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12"/>
     </row>
-    <row r="84" spans="1:1" ht="15.75" customHeight="1">
+    <row r="84" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12"/>
     </row>
-    <row r="85" spans="1:1" ht="15.75" customHeight="1">
+    <row r="85" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12"/>
     </row>
-    <row r="86" spans="1:1" ht="15.75" customHeight="1">
+    <row r="86" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12"/>
     </row>
-    <row r="87" spans="1:1" ht="15.75" customHeight="1">
+    <row r="87" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12"/>
     </row>
-    <row r="88" spans="1:1" ht="15.75" customHeight="1">
+    <row r="88" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12"/>
     </row>
-    <row r="89" spans="1:1" ht="15.75" customHeight="1">
+    <row r="89" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12"/>
     </row>
-    <row r="90" spans="1:1" ht="15.75" customHeight="1">
+    <row r="90" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12"/>
     </row>
-    <row r="91" spans="1:1" ht="15.75" customHeight="1">
+    <row r="91" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12"/>
     </row>
-    <row r="92" spans="1:1" ht="15.75" customHeight="1">
+    <row r="92" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12"/>
     </row>
-    <row r="93" spans="1:1" ht="15.75" customHeight="1">
+    <row r="93" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12"/>
     </row>
-    <row r="94" spans="1:1" ht="15.75" customHeight="1">
+    <row r="94" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12"/>
     </row>
-    <row r="95" spans="1:1" ht="15.75" customHeight="1">
+    <row r="95" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12"/>
     </row>
-    <row r="96" spans="1:1" ht="15.75" customHeight="1">
+    <row r="96" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1" ht="15.75" customHeight="1">
+    <row r="97" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1" ht="15.75" customHeight="1">
+    <row r="98" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1" ht="15.75" customHeight="1">
+    <row r="99" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1" ht="15.75" customHeight="1">
+    <row r="100" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1" ht="15.75" customHeight="1">
+    <row r="101" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="12"/>
     </row>
   </sheetData>
@@ -2547,12 +2563,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D100"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="17.28515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.42578125" customWidth="1"/>
     <col min="2" max="2" width="148.42578125" customWidth="1"/>
@@ -2560,7 +2576,7 @@
     <col min="4" max="4" width="8.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
@@ -2574,493 +2590,493 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="14"/>
       <c r="B2" s="15"/>
       <c r="C2" s="16"/>
       <c r="D2" s="17"/>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="14"/>
       <c r="B3" s="15"/>
       <c r="C3" s="16"/>
       <c r="D3" s="17"/>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="14"/>
       <c r="B4" s="15"/>
       <c r="C4" s="16"/>
       <c r="D4" s="17"/>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="18"/>
       <c r="B5" s="19"/>
       <c r="C5" s="20"/>
       <c r="D5" s="9"/>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="14"/>
       <c r="B6" s="21"/>
       <c r="C6" s="16"/>
       <c r="D6" s="17"/>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="14"/>
       <c r="B7" s="15"/>
       <c r="C7" s="16"/>
       <c r="D7" s="17"/>
     </row>
-    <row r="8" spans="1:4" ht="15.75" customHeight="1">
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="23"/>
       <c r="C8" s="12"/>
       <c r="D8" s="9"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" customHeight="1">
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="25"/>
       <c r="C9" s="12"/>
       <c r="D9" s="9"/>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1">
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="26"/>
       <c r="B10" s="27"/>
       <c r="C10" s="26"/>
       <c r="D10" s="9"/>
     </row>
-    <row r="11" spans="1:4" ht="15.75" customHeight="1">
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="26"/>
       <c r="B11" s="27"/>
       <c r="C11" s="26"/>
       <c r="D11" s="9"/>
     </row>
-    <row r="12" spans="1:4" ht="15.75" customHeight="1">
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="26"/>
       <c r="B12" s="28"/>
       <c r="C12" s="26"/>
       <c r="D12" s="9"/>
     </row>
-    <row r="13" spans="1:4" ht="15.75" customHeight="1">
+    <row r="13" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="26"/>
       <c r="B13" s="28"/>
       <c r="C13" s="26"/>
       <c r="D13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="15.75" customHeight="1">
+    <row r="14" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24"/>
       <c r="B14" s="29"/>
       <c r="C14" s="12"/>
       <c r="D14" s="9"/>
     </row>
-    <row r="15" spans="1:4" ht="15.75" customHeight="1">
+    <row r="15" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24"/>
       <c r="B15" s="29"/>
       <c r="C15" s="20"/>
       <c r="D15" s="9"/>
     </row>
-    <row r="16" spans="1:4" ht="15.75" customHeight="1">
+    <row r="16" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="26"/>
       <c r="B16" s="30"/>
       <c r="C16" s="26"/>
       <c r="D16" s="9"/>
     </row>
-    <row r="17" spans="1:4" ht="15.75" customHeight="1">
+    <row r="17" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="26"/>
       <c r="B17" s="30"/>
       <c r="C17" s="26"/>
       <c r="D17" s="9"/>
     </row>
-    <row r="18" spans="1:4" ht="15.75" customHeight="1">
+    <row r="18" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="26"/>
       <c r="B18" s="30"/>
       <c r="C18" s="26"/>
       <c r="D18" s="9"/>
     </row>
-    <row r="19" spans="1:4" ht="15.75" customHeight="1">
+    <row r="19" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="26"/>
       <c r="B19" s="30"/>
       <c r="C19" s="26"/>
       <c r="D19" s="9"/>
     </row>
-    <row r="20" spans="1:4" ht="15.75" customHeight="1">
+    <row r="20" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="26"/>
       <c r="B20" s="30"/>
       <c r="C20" s="26"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="1:4" ht="15.75" customHeight="1">
+    <row r="21" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="26"/>
       <c r="B21" s="30"/>
       <c r="C21" s="26"/>
       <c r="D21" s="9"/>
     </row>
-    <row r="22" spans="1:4" ht="15.75" customHeight="1">
+    <row r="22" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="26"/>
       <c r="B22" s="27"/>
       <c r="C22" s="26"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="15.75" customHeight="1">
+    <row r="23" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="24"/>
       <c r="B23" s="25"/>
       <c r="C23" s="20"/>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:4" ht="15.75" customHeight="1">
+    <row r="24" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="26"/>
       <c r="B24" s="27"/>
       <c r="C24" s="26"/>
       <c r="D24" s="9"/>
     </row>
-    <row r="25" spans="1:4" ht="15.75" customHeight="1">
+    <row r="25" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24"/>
       <c r="B25" s="25"/>
       <c r="C25" s="24"/>
       <c r="D25" s="9"/>
     </row>
-    <row r="26" spans="1:4" ht="15.75" customHeight="1">
+    <row r="26" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="26"/>
       <c r="B26" s="27"/>
       <c r="C26" s="12"/>
       <c r="D26" s="9"/>
     </row>
-    <row r="27" spans="1:4" ht="15.75" customHeight="1">
+    <row r="27" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="26"/>
       <c r="B27" s="27"/>
       <c r="C27" s="26"/>
       <c r="D27" s="9"/>
     </row>
-    <row r="28" spans="1:4" ht="15.75" customHeight="1">
+    <row r="28" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="26"/>
       <c r="B28" s="27"/>
       <c r="C28" s="26"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:4" ht="15.75" customHeight="1">
+    <row r="29" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="26"/>
       <c r="B29" s="27"/>
       <c r="C29" s="26"/>
       <c r="D29" s="9"/>
     </row>
-    <row r="30" spans="1:4" ht="15.75" customHeight="1">
+    <row r="30" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="26"/>
       <c r="B30" s="27"/>
       <c r="C30" s="26"/>
       <c r="D30" s="9"/>
     </row>
-    <row r="31" spans="1:4" ht="15.75" customHeight="1">
+    <row r="31" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="26"/>
       <c r="B31" s="27"/>
       <c r="C31" s="26"/>
       <c r="D31" s="9"/>
     </row>
-    <row r="32" spans="1:4" ht="15.75" customHeight="1">
+    <row r="32" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="26"/>
       <c r="B32" s="27"/>
       <c r="C32" s="26"/>
       <c r="D32" s="9"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75" customHeight="1">
+    <row r="33" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="26"/>
       <c r="B33" s="27"/>
       <c r="C33" s="26"/>
       <c r="D33" s="9"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75" customHeight="1">
+    <row r="34" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="26"/>
       <c r="B34" s="27"/>
       <c r="C34" s="26"/>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75" customHeight="1">
+    <row r="35" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="26"/>
       <c r="B35" s="27"/>
       <c r="C35" s="26"/>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75" customHeight="1">
+    <row r="36" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="26"/>
       <c r="B36" s="32"/>
       <c r="C36" s="26"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75" customHeight="1">
+    <row r="37" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="26"/>
       <c r="B37" s="32"/>
       <c r="C37" s="26"/>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75" customHeight="1">
+    <row r="38" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="26"/>
       <c r="B38" s="32"/>
       <c r="C38" s="26"/>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75" customHeight="1">
+    <row r="39" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="26"/>
       <c r="B39" s="32"/>
       <c r="C39" s="26"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75" customHeight="1">
+    <row r="40" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="26"/>
       <c r="B40" s="27"/>
       <c r="C40" s="26"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75" customHeight="1">
+    <row r="41" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="26"/>
       <c r="B41" s="32"/>
       <c r="C41" s="26"/>
       <c r="D41" s="9"/>
     </row>
-    <row r="42" spans="1:4" ht="15.75" customHeight="1">
+    <row r="42" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="26"/>
       <c r="B42" s="27"/>
       <c r="C42" s="26"/>
       <c r="D42" s="9"/>
     </row>
-    <row r="43" spans="1:4" ht="15.75" customHeight="1">
+    <row r="43" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="26"/>
       <c r="B43" s="27"/>
       <c r="C43" s="26"/>
       <c r="D43" s="9"/>
     </row>
-    <row r="44" spans="1:4" ht="15.75" customHeight="1">
+    <row r="44" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="26"/>
       <c r="B44" s="27"/>
       <c r="C44" s="26"/>
       <c r="D44" s="9"/>
     </row>
-    <row r="45" spans="1:4" ht="15.75" customHeight="1">
+    <row r="45" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="26"/>
       <c r="B45" s="27"/>
       <c r="C45" s="26"/>
       <c r="D45" s="9"/>
     </row>
-    <row r="46" spans="1:4" ht="15.75" customHeight="1">
+    <row r="46" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="26"/>
       <c r="B46" s="27"/>
       <c r="C46" s="26"/>
       <c r="D46" s="9"/>
     </row>
-    <row r="47" spans="1:4" ht="15.75" customHeight="1">
+    <row r="47" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="12"/>
       <c r="C47" s="12"/>
     </row>
-    <row r="48" spans="1:4" ht="15.75" customHeight="1">
+    <row r="48" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="26"/>
       <c r="B48" s="27"/>
       <c r="C48" s="12"/>
       <c r="D48" s="26"/>
     </row>
-    <row r="49" spans="1:4" ht="15.75" customHeight="1">
+    <row r="49" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="26"/>
       <c r="B49" s="27"/>
       <c r="C49" s="12"/>
       <c r="D49" s="26"/>
     </row>
-    <row r="50" spans="1:4" ht="15.75" customHeight="1">
+    <row r="50" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="12"/>
       <c r="C50" s="12"/>
     </row>
-    <row r="51" spans="1:4" ht="15.75" customHeight="1">
+    <row r="51" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="12"/>
       <c r="C51" s="12"/>
     </row>
-    <row r="52" spans="1:4" ht="15.75" customHeight="1">
+    <row r="52" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="12"/>
       <c r="C52" s="12"/>
     </row>
-    <row r="53" spans="1:4" ht="15.75" customHeight="1">
+    <row r="53" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12"/>
       <c r="C53" s="12"/>
     </row>
-    <row r="54" spans="1:4" ht="15.75" customHeight="1">
+    <row r="54" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="12"/>
       <c r="C54" s="12"/>
     </row>
-    <row r="55" spans="1:4" ht="15.75" customHeight="1">
+    <row r="55" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="12"/>
       <c r="C55" s="12"/>
     </row>
-    <row r="56" spans="1:4" ht="15.75" customHeight="1">
+    <row r="56" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="12"/>
       <c r="C56" s="12"/>
     </row>
-    <row r="57" spans="1:4" ht="15.75" customHeight="1">
+    <row r="57" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="12"/>
       <c r="C57" s="12"/>
     </row>
-    <row r="58" spans="1:4" ht="15.75" customHeight="1">
+    <row r="58" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="12"/>
       <c r="C58" s="12"/>
     </row>
-    <row r="59" spans="1:4" ht="15.75" customHeight="1">
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="12"/>
       <c r="C59" s="12"/>
     </row>
-    <row r="60" spans="1:4" ht="15.75" customHeight="1">
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="12"/>
       <c r="C60" s="12"/>
     </row>
-    <row r="61" spans="1:4" ht="15.75" customHeight="1">
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="12"/>
       <c r="C61" s="12"/>
     </row>
-    <row r="62" spans="1:4" ht="15.75" customHeight="1">
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="12"/>
       <c r="C62" s="12"/>
     </row>
-    <row r="63" spans="1:4" ht="15.75" customHeight="1">
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="12"/>
       <c r="C63" s="12"/>
     </row>
-    <row r="64" spans="1:4" ht="15.75" customHeight="1">
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="12"/>
       <c r="C64" s="12"/>
     </row>
-    <row r="65" spans="1:3" ht="15.75" customHeight="1">
+    <row r="65" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="12"/>
       <c r="C65" s="12"/>
     </row>
-    <row r="66" spans="1:3" ht="15.75" customHeight="1">
+    <row r="66" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="12"/>
       <c r="C66" s="12"/>
     </row>
-    <row r="67" spans="1:3" ht="15.75" customHeight="1">
+    <row r="67" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="12"/>
       <c r="C67" s="12"/>
     </row>
-    <row r="68" spans="1:3" ht="15.75" customHeight="1">
+    <row r="68" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="12"/>
       <c r="C68" s="12"/>
     </row>
-    <row r="69" spans="1:3" ht="15.75" customHeight="1">
+    <row r="69" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="12"/>
       <c r="C69" s="12"/>
     </row>
-    <row r="70" spans="1:3" ht="15.75" customHeight="1">
+    <row r="70" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="12"/>
       <c r="C70" s="12"/>
     </row>
-    <row r="71" spans="1:3" ht="15.75" customHeight="1">
+    <row r="71" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="12"/>
       <c r="C71" s="12"/>
     </row>
-    <row r="72" spans="1:3" ht="15.75" customHeight="1">
+    <row r="72" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="12"/>
       <c r="C72" s="12"/>
     </row>
-    <row r="73" spans="1:3" ht="15.75" customHeight="1">
+    <row r="73" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="12"/>
       <c r="C73" s="12"/>
     </row>
-    <row r="74" spans="1:3" ht="15.75" customHeight="1">
+    <row r="74" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="12"/>
       <c r="C74" s="12"/>
     </row>
-    <row r="75" spans="1:3" ht="15.75" customHeight="1">
+    <row r="75" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="12"/>
       <c r="C75" s="12"/>
     </row>
-    <row r="76" spans="1:3" ht="15.75" customHeight="1">
+    <row r="76" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="12"/>
       <c r="C76" s="12"/>
     </row>
-    <row r="77" spans="1:3" ht="15.75" customHeight="1">
+    <row r="77" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="12"/>
       <c r="C77" s="12"/>
     </row>
-    <row r="78" spans="1:3" ht="15.75" customHeight="1">
+    <row r="78" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12"/>
       <c r="C78" s="12"/>
     </row>
-    <row r="79" spans="1:3" ht="15.75" customHeight="1">
+    <row r="79" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="12"/>
       <c r="C79" s="12"/>
     </row>
-    <row r="80" spans="1:3" ht="15.75" customHeight="1">
+    <row r="80" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="12"/>
       <c r="C80" s="12"/>
     </row>
-    <row r="81" spans="1:3" ht="15.75" customHeight="1">
+    <row r="81" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="12"/>
       <c r="C81" s="12"/>
     </row>
-    <row r="82" spans="1:3" ht="15.75" customHeight="1">
+    <row r="82" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="12"/>
       <c r="C82" s="12"/>
     </row>
-    <row r="83" spans="1:3" ht="15.75" customHeight="1">
+    <row r="83" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="12"/>
       <c r="C83" s="12"/>
     </row>
-    <row r="84" spans="1:3" ht="15.75" customHeight="1">
+    <row r="84" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="12"/>
       <c r="C84" s="12"/>
     </row>
-    <row r="85" spans="1:3" ht="15.75" customHeight="1">
+    <row r="85" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="12"/>
       <c r="C85" s="12"/>
     </row>
-    <row r="86" spans="1:3" ht="15.75" customHeight="1">
+    <row r="86" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="12"/>
       <c r="C86" s="12"/>
     </row>
-    <row r="87" spans="1:3" ht="15.75" customHeight="1">
+    <row r="87" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="12"/>
       <c r="C87" s="12"/>
     </row>
-    <row r="88" spans="1:3" ht="15.75" customHeight="1">
+    <row r="88" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="12"/>
       <c r="C88" s="12"/>
     </row>
-    <row r="89" spans="1:3" ht="15.75" customHeight="1">
+    <row r="89" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="12"/>
       <c r="C89" s="12"/>
     </row>
-    <row r="90" spans="1:3" ht="15.75" customHeight="1">
+    <row r="90" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="12"/>
       <c r="C90" s="12"/>
     </row>
-    <row r="91" spans="1:3" ht="15.75" customHeight="1">
+    <row r="91" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="12"/>
       <c r="C91" s="12"/>
     </row>
-    <row r="92" spans="1:3" ht="15.75" customHeight="1">
+    <row r="92" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="12"/>
       <c r="C92" s="12"/>
     </row>
-    <row r="93" spans="1:3" ht="15.75" customHeight="1">
+    <row r="93" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="12"/>
       <c r="C93" s="12"/>
     </row>
-    <row r="94" spans="1:3" ht="15.75" customHeight="1">
+    <row r="94" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12"/>
       <c r="C94" s="12"/>
     </row>
-    <row r="95" spans="1:3" ht="15.75" customHeight="1">
+    <row r="95" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="12"/>
       <c r="C95" s="12"/>
     </row>
-    <row r="96" spans="1:3" ht="15.75" customHeight="1">
+    <row r="96" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="12"/>
       <c r="C96" s="12"/>
     </row>
-    <row r="97" spans="1:3" ht="15.75" customHeight="1">
+    <row r="97" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="12"/>
       <c r="C97" s="12"/>
     </row>
-    <row r="98" spans="1:3" ht="15.75" customHeight="1">
+    <row r="98" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="12"/>
       <c r="C98" s="12"/>
     </row>
-    <row r="99" spans="1:3" ht="15.75" customHeight="1">
+    <row r="99" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="12"/>
       <c r="C99" s="12"/>
     </row>
-    <row r="100" spans="1:3" ht="15.75" customHeight="1">
+    <row r="100" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="12"/>
       <c r="C100" s="12"/>
     </row>

</xml_diff>